<commit_message>
Modified Lights group file.
</commit_message>
<xml_diff>
--- a/Device Interaction/Automation/Lights.xlsx
+++ b/Device Interaction/Automation/Lights.xlsx
@@ -119,11 +119,24 @@
         <t xml:space="preserve">If the drawer is open the app send the notification. If the drawer is still open for another 60 minutes, the app will send another notification. After 10 minutes if the drawer is still open, the red light will turn on.</t>
       </text>
     </comment>
+    <comment authorId="0" ref="E4">
+      <text>
+        <t xml:space="preserve">Lock vs. Lock/Unlock -&gt; There should be a conflict between lock and unlock events!
+----
+Analysis is not sure about this but actually they have no conflict.
+	-Rahmadi Trimananda</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="D5">
       <text>
         <t xml:space="preserve">If the temperature is not good, it will notify the user to move its medicine. If the user did not move them in 60 minutes, again it will notify the user. After extra 10 minutes, it will turn on the red light.</t>
       </text>
     </comment>
+    <comment authorId="0" ref="E5">
+      <text>
+        <t xml:space="preserve">Lock vs. Lock/Unlock -&gt; There should be a conflict between lock and unlock events!</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="G5">
       <text>
         <t xml:space="preserve">Lock vs. Lock/Unlock -&gt; There should be a conflict between lock and unlock events!</t>
@@ -137,16 +150,6 @@
     <comment authorId="0" ref="D7">
       <text>
         <t xml:space="preserve">Change the color of the light according to daylight. (Sunset and sunrise time)</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="E7">
-      <text>
-        <t xml:space="preserve">Lock vs. Lock/Unlock -&gt; There should be a conflict between lock and unlock events!</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="G7">
-      <text>
-        <t xml:space="preserve">Lock vs. Lock/Unlock -&gt; There should be a conflict between lock and unlock events!</t>
       </text>
     </comment>
     <comment authorId="0" ref="D8">
@@ -201,12 +204,6 @@
       <text>
         <t xml:space="preserve">The door will never be locked after x minutes that it is closed. (A person might be in the sense of presence sensor.)
 ==&gt; "We want the room to be locked after x minutes."</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="E4">
-      <text>
-        <t xml:space="preserve">Analysis is not sure about this but actually they have no conflict.
-	-Rahmadi Trimananda</t>
       </text>
     </comment>
   </commentList>
@@ -216,15 +213,33 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="34">
   <si>
+    <t>Features</t>
+  </si>
+  <si>
     <t>Application</t>
   </si>
   <si>
+    <t>door-state-to-color-light-hue-bulb.groovy</t>
+  </si>
+  <si>
+    <t>hue-minimote.groovy</t>
+  </si>
+  <si>
+    <t>hue-mood-lighting.groovy</t>
+  </si>
+  <si>
+    <t>notify-me-with-hue.groovy</t>
+  </si>
+  <si>
+    <t>step-notifier.groovy</t>
+  </si>
+  <si>
+    <t>BetterLaundryMonitor.groovy</t>
+  </si>
+  <si>
     <t>color-coordinator.groovy</t>
   </si>
   <si>
-    <t>Features</t>
-  </si>
-  <si>
     <t>initial-state-event-streamer.groovy</t>
   </si>
   <si>
@@ -252,24 +267,6 @@
     <t>unbuffered-event-sender.groovy</t>
   </si>
   <si>
-    <t>door-state-to-color-light-hue-bulb.groovy</t>
-  </si>
-  <si>
-    <t>hue-minimote.groovy</t>
-  </si>
-  <si>
-    <t>hue-mood-lighting.groovy</t>
-  </si>
-  <si>
-    <t>notify-me-with-hue.groovy</t>
-  </si>
-  <si>
-    <t>step-notifier.groovy</t>
-  </si>
-  <si>
-    <t>BetterLaundryMonitor.groovy</t>
-  </si>
-  <si>
     <t>Hue Party Mode.groovy</t>
   </si>
   <si>
@@ -294,19 +291,19 @@
     <t>setColor</t>
   </si>
   <si>
+    <t>timeout</t>
+  </si>
+  <si>
     <t>detected</t>
   </si>
   <si>
     <t>manual/sensor</t>
   </si>
   <si>
-    <t>timeout</t>
+    <t>oom</t>
   </si>
   <si>
     <t>manual/schedule</t>
-  </si>
-  <si>
-    <t>oom</t>
   </si>
   <si>
     <t>no error</t>
@@ -346,6 +343,11 @@
       <name val="Arial"/>
     </font>
     <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
     </font>
     <font>
@@ -362,11 +364,6 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -418,14 +415,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
-        <bgColor rgb="FF00FF00"/>
+        <fgColor rgb="FF4A86E8"/>
+        <bgColor rgb="FF4A86E8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4A86E8"/>
-        <bgColor rgb="FF4A86E8"/>
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -452,16 +449,16 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -481,46 +478,46 @@
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="9" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="6" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -529,12 +526,15 @@
     <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="8" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="9" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
@@ -559,9 +559,6 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="9" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="6" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -635,29 +632,29 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>16</v>
+      <c r="G1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>18</v>
@@ -680,32 +677,32 @@
       <c r="D2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="12" t="str">
+      <c r="E2" s="13" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/official/door-state-to-color-light-hue-bulb.groovy","door-state-to-color-light-hue-bulb.groovy")</f>
         <v>door-state-to-color-light-hue-bulb.groovy</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="13" t="s">
+      <c r="F2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -726,28 +723,28 @@
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/official/hue-minimote.groovy","hue-minimote.groovy")</f>
         <v>hue-minimote.groovy</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="13" t="s">
+      <c r="F3" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -759,37 +756,37 @@
         <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="12" t="str">
+      <c r="E4" s="13" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/official/hue-mood-lighting.groovy","hue-mood-lighting.groovy")</f>
         <v>hue-mood-lighting.groovy</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="13" t="s">
+      <c r="F4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -801,7 +798,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>25</v>
@@ -810,28 +807,28 @@
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/official/notify-me-with-hue.groovy","notify-me-with-hue.groovy")</f>
         <v>notify-me-with-hue.groovy</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="13" t="s">
+      <c r="F5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -852,28 +849,28 @@
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/official/step-notifier.groovy","step-notifier.groovy")</f>
         <v>step-notifier.groovy</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="13" t="s">
+      <c r="F6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -890,32 +887,32 @@
       <c r="D7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="12" t="str">
+      <c r="E7" s="13" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/third-party/BetterLaundryMonitor.groovy","BetterLaundryMonitor.groovy")</f>
         <v>BetterLaundryMonitor.groovy</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="13" t="s">
+      <c r="F7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -927,37 +924,37 @@
         <v>19</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="19" t="str">
+      <c r="E8" s="20" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/third-party/Hue-Party-Mode.groovy","Hue Party Mode.groovy")</f>
         <v>Hue Party Mode.groovy</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="13" t="s">
+      <c r="I8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -965,48 +962,48 @@
       <c r="A9" s="9">
         <v>8.0</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="22" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="22" t="str">
+      <c r="E9" s="23" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/official/mini-hue-controller.groovy","mini-hue-controller.groovy")</f>
         <v>mini-hue-controller.groovy</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="I9" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="L9" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="M9" s="13" t="s">
+      <c r="M9" s="12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1"/>
       <c r="E10" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="8">
         <f>countif(F$2:F$9, "detected")</f>
@@ -1044,7 +1041,7 @@
         <f t="shared" ref="N10:N13" si="3">sum(F10:M10)</f>
         <v>23</v>
       </c>
-      <c r="O10" s="21" t="s">
+      <c r="O10" s="22" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1093,7 +1090,7 @@
     <row r="12">
       <c r="A12" s="1"/>
       <c r="E12" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="8">
         <f>COUNTIF(F$2:F$9, "oom")</f>
@@ -1138,7 +1135,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F13" s="8">
         <f>COUNTIF(F$2:F$9, "timeout")</f>
@@ -1192,11 +1189,11 @@
     </row>
     <row r="15">
       <c r="A15" s="1"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="G15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="G15" s="31"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1205,11 +1202,11 @@
     </row>
     <row r="16">
       <c r="A16" s="1"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="G16" s="31"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="G16" s="34"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1218,11 +1215,11 @@
     </row>
     <row r="17">
       <c r="A17" s="1"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="G17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="G17" s="35"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1231,11 +1228,11 @@
     </row>
     <row r="18">
       <c r="A18" s="1"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="G18" s="31"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="G18" s="34"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1244,11 +1241,11 @@
     </row>
     <row r="19">
       <c r="A19" s="1"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="G19" s="31"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="G19" s="34"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1257,11 +1254,11 @@
     </row>
     <row r="20">
       <c r="A20" s="1"/>
-      <c r="B20" s="33"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="G20" s="32"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1283,11 +1280,11 @@
     </row>
     <row r="22">
       <c r="A22" s="1"/>
-      <c r="B22" s="28"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="G22" s="29"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="G22" s="31"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -1296,11 +1293,11 @@
     </row>
     <row r="23">
       <c r="A23" s="1"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="G23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="G23" s="34"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1310,10 +1307,10 @@
     <row r="24">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="G24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="G24" s="34"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1322,11 +1319,11 @@
     </row>
     <row r="25">
       <c r="A25" s="1"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="G25" s="31"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="G25" s="34"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -1335,11 +1332,11 @@
     </row>
     <row r="26">
       <c r="A26" s="1"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="G26" s="32"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="G26" s="35"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -1347,18 +1344,18 @@
       <c r="L26" s="1"/>
     </row>
     <row r="27">
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="G27" s="29"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="G27" s="31"/>
     </row>
     <row r="28">
-      <c r="B28" s="28"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="G28" s="31"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="G28" s="34"/>
     </row>
     <row r="29">
       <c r="B29" s="1"/>
@@ -1368,31 +1365,31 @@
       <c r="F29" s="1"/>
     </row>
     <row r="32">
-      <c r="G32" s="36"/>
+      <c r="G32" s="39"/>
     </row>
     <row r="33">
-      <c r="G33" s="2"/>
-      <c r="I33" s="37"/>
+      <c r="G33" s="5"/>
+      <c r="I33" s="40"/>
     </row>
     <row r="34">
-      <c r="G34" s="2"/>
-      <c r="I34" s="37"/>
+      <c r="G34" s="5"/>
+      <c r="I34" s="40"/>
     </row>
     <row r="35">
-      <c r="G35" s="2"/>
-      <c r="I35" s="37"/>
+      <c r="G35" s="5"/>
+      <c r="I35" s="40"/>
     </row>
     <row r="36">
-      <c r="G36" s="2"/>
-      <c r="I36" s="37"/>
+      <c r="G36" s="5"/>
+      <c r="I36" s="40"/>
     </row>
     <row r="37">
-      <c r="G37" s="2"/>
-      <c r="I37" s="37"/>
+      <c r="G37" s="5"/>
+      <c r="I37" s="40"/>
     </row>
     <row r="38">
-      <c r="G38" s="2"/>
-      <c r="I38" s="37"/>
+      <c r="G38" s="5"/>
+      <c r="I38" s="40"/>
     </row>
     <row r="39">
       <c r="G39" s="1"/>
@@ -1465,38 +1462,38 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="O1" s="7" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/official/hue-minimote.groovy","hue-minimote.groovy")</f>
@@ -1517,37 +1514,37 @@
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/official/color-coordinator.groovy","color-coordinator.groovy")</f>
         <v>color-coordinator.groovy</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="13" t="s">
+      <c r="E2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1561,41 +1558,41 @@
       <c r="C3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="16" t="str">
+      <c r="D3" s="15" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/official/initial-state-event-streamer.groovy","initial-state-event-streamer.groovy")</f>
         <v>initial-state-event-streamer.groovy</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="13" t="s">
+      <c r="E3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1613,37 +1610,37 @@
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/official/medicine-management-contact-sensor.groovy","medicine-management-contact-sensor.groovy")</f>
         <v>medicine-management-contact-sensor.groovy</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" s="13" t="s">
+      <c r="E4" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1661,37 +1658,37 @@
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/official/medicine-management-temp-motion.groovy","medicine-management-temp-motion.groovy")</f>
         <v>medicine-management-temp-motion.groovy</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O5" s="13" t="s">
+      <c r="E5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1705,41 +1702,41 @@
       <c r="C6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="16" t="str">
+      <c r="D6" s="15" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/third-party/buffered-event-sender.groovy","buffered-event-sender.groovy")</f>
         <v>buffered-event-sender.groovy</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O6" s="13" t="s">
+      <c r="E6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1753,41 +1750,41 @@
       <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="24" t="str">
+      <c r="D7" s="18" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/third-party/circadian-daylight.groovy","circadian-daylight.groovy")</f>
         <v>circadian-daylight.groovy</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="15" t="s">
+      <c r="F7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" s="13" t="s">
+      <c r="H7" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1801,41 +1798,41 @@
       <c r="C8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="16" t="str">
+      <c r="D8" s="15" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/third-party/influxdb-logger.groovy","influxdb-logger.groovy")</f>
         <v>influxdb-logger.groovy</v>
       </c>
-      <c r="E8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8" s="13" t="s">
+      <c r="E8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1849,41 +1846,41 @@
       <c r="C9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="16" t="str">
+      <c r="D9" s="15" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/third-party/initial-state-event-sender.groovy","initial-state-event-sender.groovy")</f>
         <v>initial-state-event-sender.groovy</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" s="13" t="s">
+      <c r="E9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1897,41 +1894,41 @@
       <c r="C10" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="16" t="str">
+      <c r="D10" s="15" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/third-party/initial-state-event-sender.groovy","initialstate-smart-app-v1.2.0.groovy")</f>
         <v>initialstate-smart-app-v1.2.0.groovy</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O10" s="13" t="s">
+      <c r="E10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1945,41 +1942,41 @@
       <c r="C11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="16" t="str">
+      <c r="D11" s="15" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/third-party/unbuffered-event-sender.groovy","unbuffered-event-sender.groovy")</f>
         <v>unbuffered-event-sender.groovy</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="N11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O11" s="13" t="s">
+      <c r="E11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1987,47 +1984,47 @@
       <c r="A12" s="10">
         <v>11.0</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="22" t="str">
+      <c r="D12" s="23" t="str">
         <f>HYPERLINK("https://github.uci.edu/rtrimana/smartthings_app/blob/master/official/hue-minimote.groovy","hue-minimote.groovy")</f>
         <v>hue-minimote.groovy</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="M12" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="O12" s="13" t="s">
+      <c r="E12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="12" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2036,11 +2033,11 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="8">
         <f>countif(E$2:E$12, "detected")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" ref="F13:O13" si="1">countif(F2:F12, "detected")</f>
@@ -2048,7 +2045,7 @@
       </c>
       <c r="G13" s="10">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H13" s="10">
         <f t="shared" si="1"/>
@@ -2082,7 +2079,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P13" s="38">
+      <c r="P13" s="28">
         <f t="shared" ref="P13:P16" si="3">sum(E13:O13)</f>
         <v>7</v>
       </c>
@@ -2138,7 +2135,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P14" s="39">
+      <c r="P14" s="29">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -2148,7 +2145,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" s="8">
         <f t="shared" ref="E15:O15" si="4">COUNTIF(E$2:E$12, "oom")</f>
@@ -2194,7 +2191,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P15" s="40">
+      <c r="P15" s="32">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
@@ -2204,11 +2201,11 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E16" s="8">
         <f t="shared" ref="E16:O16" si="5">COUNTIF(E$2:E$12, "timeout")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" s="8">
         <f t="shared" si="5"/>
@@ -2216,7 +2213,7 @@
       </c>
       <c r="G16" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="8">
         <f t="shared" si="5"/>
@@ -2250,7 +2247,7 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="P16" s="40">
+      <c r="P16" s="32">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
@@ -2260,7 +2257,7 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="36"/>
+      <c r="E17" s="39"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -2277,7 +2274,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="36"/>
+      <c r="E18" s="39"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -2294,7 +2291,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="36"/>
+      <c r="E19" s="39"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2343,10 +2340,10 @@
     <row r="22">
       <c r="A22" s="1"/>
       <c r="B22" s="42"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="29"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2360,14 +2357,14 @@
     <row r="23">
       <c r="A23" s="1"/>
       <c r="B23" s="43"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="31"/>
+      <c r="F23" s="34"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="29"/>
+      <c r="J23" s="31"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -2378,13 +2375,13 @@
       <c r="A24" s="1"/>
       <c r="B24" s="43"/>
       <c r="C24" s="44"/>
-      <c r="D24" s="29"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="31"/>
+      <c r="F24" s="34"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="29"/>
+      <c r="J24" s="31"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -2397,11 +2394,11 @@
       <c r="C25" s="44"/>
       <c r="D25" s="44"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="31"/>
+      <c r="F25" s="34"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="46"/>
-      <c r="J25" s="29"/>
+      <c r="J25" s="31"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -2411,10 +2408,10 @@
     <row r="26">
       <c r="A26" s="1"/>
       <c r="B26" s="47"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="31"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="46"/>
@@ -2429,9 +2426,9 @@
       <c r="A27" s="1"/>
       <c r="B27" s="45"/>
       <c r="C27" s="44"/>
-      <c r="D27" s="29"/>
+      <c r="D27" s="31"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="31"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -2462,10 +2459,10 @@
     <row r="29">
       <c r="A29" s="1"/>
       <c r="B29" s="42"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="29"/>
+      <c r="F29" s="31"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -2482,7 +2479,7 @@
       <c r="C30" s="44"/>
       <c r="D30" s="44"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="31"/>
+      <c r="F30" s="34"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -2499,7 +2496,7 @@
       <c r="C31" s="44"/>
       <c r="D31" s="44"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="31"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -2513,10 +2510,10 @@
     <row r="32">
       <c r="A32" s="1"/>
       <c r="B32" s="49"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -2530,10 +2527,10 @@
     <row r="33">
       <c r="A33" s="1"/>
       <c r="B33" s="50"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -2545,11 +2542,11 @@
       <c r="O33" s="1"/>
     </row>
     <row r="34">
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="29"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -2562,10 +2559,10 @@
     </row>
     <row r="35">
       <c r="B35" s="42"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -2644,7 +2641,7 @@
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="36"/>
+      <c r="E40" s="39"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -2660,8 +2657,8 @@
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="2"/>
-      <c r="G41" s="37"/>
+      <c r="E41" s="5"/>
+      <c r="G41" s="40"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
@@ -2675,8 +2672,8 @@
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="2"/>
-      <c r="G42" s="37"/>
+      <c r="E42" s="5"/>
+      <c r="G42" s="40"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -2690,8 +2687,8 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="2"/>
-      <c r="G43" s="37"/>
+      <c r="E43" s="5"/>
+      <c r="G43" s="40"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -2705,8 +2702,8 @@
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="2"/>
-      <c r="G44" s="37"/>
+      <c r="E44" s="5"/>
+      <c r="G44" s="40"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
@@ -2717,12 +2714,12 @@
       <c r="O44" s="1"/>
     </row>
     <row r="45">
-      <c r="E45" s="2"/>
-      <c r="G45" s="37"/>
+      <c r="E45" s="5"/>
+      <c r="G45" s="40"/>
     </row>
     <row r="46">
-      <c r="E46" s="2"/>
-      <c r="G46" s="37"/>
+      <c r="E46" s="5"/>
+      <c r="G46" s="40"/>
     </row>
     <row r="48">
       <c r="B48" s="1"/>

</xml_diff>